<commit_message>
Update data files (exclude secrets)
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\py\7s\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8347D3D3-48E4-4D7F-A585-CABC9E6E0C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EA67DE-BFD6-4125-8081-363F426192A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="343">
   <si>
     <t>الاسم</t>
   </si>
@@ -1051,6 +1051,9 @@
   </si>
   <si>
     <t>000r</t>
+  </si>
+  <si>
+    <t>Hmw14232002</t>
   </si>
 </sst>
 </file>
@@ -1433,7 +1436,7 @@
   <dimension ref="A1:K143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2025,7 +2028,7 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>342</v>
       </c>
       <c r="D19" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Full project update: all files and folders
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\py\7s\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FABAF6-9E7B-40FD-94C8-686BD146A7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0AA89C-F93B-4E61-81B3-F2FC571ABBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="344">
   <si>
     <t>الاسم</t>
   </si>
@@ -192,6 +192,9 @@
     <t>المواردالبشريه</t>
   </si>
   <si>
+    <t>000r</t>
+  </si>
+  <si>
     <t>razaan-alahmadi@sevens.sa</t>
   </si>
   <si>
@@ -228,12 +231,12 @@
     <t>حسان محمد وصل الله الحربي</t>
   </si>
   <si>
+    <t>Hmw14232002</t>
+  </si>
+  <si>
     <t>hassan-alharbi@sevens.sa</t>
   </si>
   <si>
-    <t>requests,rental,maintenance,stock,warehouse</t>
-  </si>
-  <si>
     <t xml:space="preserve">محمد نور الشبلي  </t>
   </si>
   <si>
@@ -1050,17 +1053,17 @@
     <t>requests,rental,maintenance,stock</t>
   </si>
   <si>
-    <t>000r</t>
-  </si>
-  <si>
-    <t>Hmw14232002</t>
+    <t>requests,rental,maintenance,warehouse,periodic_maintenance</t>
+  </si>
+  <si>
+    <t>warehouse,requests,periodic_maintenance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1072,20 +1075,6 @@
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1120,19 +1109,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1435,11 +1421,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="53.625" customWidth="1"/>
+    <col min="9" max="9" width="61.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1495,11 +1485,11 @@
       <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="G2">
-        <v>1</v>
+      <c r="G2" t="s">
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>343</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
@@ -1531,7 +1521,7 @@
         <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>343</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
@@ -1559,8 +1549,8 @@
       <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="G4">
-        <v>1</v>
+      <c r="G4" t="s">
+        <v>17</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -1900,19 +1890,19 @@
         <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>341</v>
-      </c>
-      <c r="D15" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
       </c>
-      <c r="G15">
-        <v>0</v>
+      <c r="G15" t="s">
+        <v>17</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
@@ -1926,7 +1916,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
         <v>54</v>
@@ -1934,17 +1924,17 @@
       <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>58</v>
+      <c r="D16" t="s">
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
       </c>
-      <c r="G16">
-        <v>1</v>
+      <c r="G16" t="s">
+        <v>24</v>
       </c>
       <c r="I16" t="s">
         <v>18</v>
@@ -1958,7 +1948,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
@@ -1967,10 +1957,10 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -1990,7 +1980,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
@@ -1998,11 +1988,11 @@
       <c r="C18" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>64</v>
+      <c r="D18" t="s">
+        <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -2022,28 +2012,28 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" t="s">
         <v>66</v>
       </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" t="s">
         <v>342</v>
-      </c>
-      <c r="D19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>68</v>
       </c>
       <c r="J19" t="s">
         <v>19</v>
@@ -2054,7 +2044,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
@@ -2063,10 +2053,10 @@
         <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
         <v>16</v>
@@ -2086,7 +2076,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
         <v>30</v>
@@ -2095,16 +2085,16 @@
         <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F21" t="s">
         <v>16</v>
       </c>
-      <c r="G21">
-        <v>1</v>
+      <c r="G21" t="s">
+        <v>24</v>
       </c>
       <c r="I21" t="s">
         <v>18</v>
@@ -2118,25 +2108,25 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
         <v>74</v>
       </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" t="s">
-        <v>73</v>
-      </c>
       <c r="F22" t="s">
         <v>16</v>
       </c>
-      <c r="G22">
-        <v>1</v>
+      <c r="G22" t="s">
+        <v>24</v>
       </c>
       <c r="I22" t="s">
         <v>18</v>
@@ -2150,7 +2140,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -2159,10 +2149,10 @@
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
         <v>16</v>
@@ -2182,7 +2172,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -2191,16 +2181,16 @@
         <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F24" t="s">
         <v>16</v>
       </c>
-      <c r="G24">
-        <v>1</v>
+      <c r="G24" t="s">
+        <v>17</v>
       </c>
       <c r="I24" t="s">
         <v>18</v>
@@ -2214,7 +2204,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -2223,10 +2213,10 @@
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F25" t="s">
         <v>16</v>
@@ -2246,7 +2236,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
         <v>30</v>
@@ -2255,10 +2245,10 @@
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F26" t="s">
         <v>16</v>
@@ -2278,19 +2268,19 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" t="s">
         <v>85</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" t="s">
-        <v>84</v>
       </c>
       <c r="F27" t="s">
         <v>16</v>
@@ -2310,7 +2300,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -2319,10 +2309,10 @@
         <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F28" t="s">
         <v>16</v>
@@ -2342,7 +2332,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
@@ -2351,10 +2341,10 @@
         <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F29" t="s">
         <v>16</v>
@@ -2374,7 +2364,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
@@ -2383,10 +2373,10 @@
         <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F30" t="s">
         <v>16</v>
@@ -2406,7 +2396,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
         <v>26</v>
@@ -2415,10 +2405,10 @@
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E31" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F31" t="s">
         <v>16</v>
@@ -2438,7 +2428,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
         <v>26</v>
@@ -2447,10 +2437,10 @@
         <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F32" t="s">
         <v>16</v>
@@ -2470,7 +2460,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
         <v>26</v>
@@ -2479,10 +2469,10 @@
         <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F33" t="s">
         <v>16</v>
@@ -2502,7 +2492,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
         <v>26</v>
@@ -2511,10 +2501,10 @@
         <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E34" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s">
         <v>16</v>
@@ -2534,7 +2524,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B35" t="s">
         <v>26</v>
@@ -2543,10 +2533,10 @@
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F35" t="s">
         <v>16</v>
@@ -2566,7 +2556,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
         <v>26</v>
@@ -2575,10 +2565,10 @@
         <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F36" t="s">
         <v>16</v>
@@ -2598,7 +2588,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
         <v>26</v>
@@ -2607,10 +2597,10 @@
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F37" t="s">
         <v>16</v>
@@ -2630,7 +2620,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B38" t="s">
         <v>26</v>
@@ -2639,10 +2629,10 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E38" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F38" t="s">
         <v>16</v>
@@ -2662,7 +2652,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
         <v>26</v>
@@ -2671,10 +2661,10 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F39" t="s">
         <v>16</v>
@@ -2694,7 +2684,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B40" t="s">
         <v>26</v>
@@ -2703,10 +2693,10 @@
         <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E40" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F40" t="s">
         <v>16</v>
@@ -2726,7 +2716,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B41" t="s">
         <v>26</v>
@@ -2735,10 +2725,10 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E41" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F41" t="s">
         <v>16</v>
@@ -2758,7 +2748,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B42" t="s">
         <v>26</v>
@@ -2767,10 +2757,10 @@
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F42" t="s">
         <v>16</v>
@@ -2790,7 +2780,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B43" t="s">
         <v>26</v>
@@ -2799,10 +2789,10 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F43" t="s">
         <v>16</v>
@@ -2822,7 +2812,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B44" t="s">
         <v>26</v>
@@ -2831,10 +2821,10 @@
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E44" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F44" t="s">
         <v>16</v>
@@ -2854,7 +2844,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B45" t="s">
         <v>26</v>
@@ -2863,10 +2853,10 @@
         <v>13</v>
       </c>
       <c r="D45" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E45" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F45" t="s">
         <v>16</v>
@@ -2886,7 +2876,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B46" t="s">
         <v>26</v>
@@ -2895,10 +2885,10 @@
         <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F46" t="s">
         <v>16</v>
@@ -2918,7 +2908,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B47" t="s">
         <v>26</v>
@@ -2927,10 +2917,10 @@
         <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F47" t="s">
         <v>16</v>
@@ -2950,7 +2940,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B48" t="s">
         <v>26</v>
@@ -2959,10 +2949,10 @@
         <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F48" t="s">
         <v>16</v>
@@ -2982,7 +2972,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
         <v>26</v>
@@ -2991,10 +2981,10 @@
         <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E49" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F49" t="s">
         <v>16</v>
@@ -3014,7 +3004,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B50" t="s">
         <v>26</v>
@@ -3023,10 +3013,10 @@
         <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E50" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F50" t="s">
         <v>16</v>
@@ -3046,7 +3036,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
         <v>26</v>
@@ -3055,10 +3045,10 @@
         <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E51" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F51" t="s">
         <v>16</v>
@@ -3078,7 +3068,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B52" t="s">
         <v>26</v>
@@ -3087,10 +3077,10 @@
         <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E52" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F52" t="s">
         <v>16</v>
@@ -3110,7 +3100,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B53" t="s">
         <v>26</v>
@@ -3122,7 +3112,7 @@
         <v>39</v>
       </c>
       <c r="E53" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F53" t="s">
         <v>16</v>
@@ -3142,19 +3132,19 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B54" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C54" t="s">
         <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E54" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F54" t="s">
         <v>16</v>
@@ -3163,7 +3153,7 @@
         <v>24</v>
       </c>
       <c r="H54" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I54" t="s">
         <v>18</v>
@@ -3177,7 +3167,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B55" t="s">
         <v>26</v>
@@ -3186,10 +3176,10 @@
         <v>13</v>
       </c>
       <c r="D55" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E55" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F55" t="s">
         <v>16</v>
@@ -3209,7 +3199,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B56" t="s">
         <v>26</v>
@@ -3218,10 +3208,10 @@
         <v>13</v>
       </c>
       <c r="D56" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E56" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F56" t="s">
         <v>16</v>
@@ -3241,7 +3231,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B57" t="s">
         <v>26</v>
@@ -3253,7 +3243,7 @@
         <v>39</v>
       </c>
       <c r="E57" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F57" t="s">
         <v>16</v>
@@ -3273,7 +3263,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
         <v>26</v>
@@ -3282,10 +3272,10 @@
         <v>13</v>
       </c>
       <c r="D58" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E58" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F58" t="s">
         <v>16</v>
@@ -3305,19 +3295,19 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>153</v>
+      </c>
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" t="s">
+        <v>154</v>
+      </c>
+      <c r="E59" t="s">
         <v>152</v>
-      </c>
-      <c r="B59" t="s">
-        <v>26</v>
-      </c>
-      <c r="C59" t="s">
-        <v>13</v>
-      </c>
-      <c r="D59" t="s">
-        <v>153</v>
-      </c>
-      <c r="E59" t="s">
-        <v>151</v>
       </c>
       <c r="F59" t="s">
         <v>16</v>
@@ -3337,7 +3327,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B60" t="s">
         <v>26</v>
@@ -3346,10 +3336,10 @@
         <v>13</v>
       </c>
       <c r="D60" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E60" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F60" t="s">
         <v>16</v>
@@ -3369,7 +3359,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B61" t="s">
         <v>26</v>
@@ -3378,10 +3368,10 @@
         <v>13</v>
       </c>
       <c r="D61" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E61" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F61" t="s">
         <v>16</v>
@@ -3401,7 +3391,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B62" t="s">
         <v>26</v>
@@ -3410,10 +3400,10 @@
         <v>13</v>
       </c>
       <c r="D62" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E62" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F62" t="s">
         <v>16</v>
@@ -3433,7 +3423,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B63" t="s">
         <v>26</v>
@@ -3442,10 +3432,10 @@
         <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E63" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F63" t="s">
         <v>16</v>
@@ -3465,7 +3455,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B64" t="s">
         <v>26</v>
@@ -3474,10 +3464,10 @@
         <v>13</v>
       </c>
       <c r="D64" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E64" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F64" t="s">
         <v>16</v>
@@ -3497,7 +3487,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B65" t="s">
         <v>26</v>
@@ -3506,10 +3496,10 @@
         <v>13</v>
       </c>
       <c r="D65" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E65" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F65" t="s">
         <v>16</v>
@@ -3529,7 +3519,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B66" t="s">
         <v>26</v>
@@ -3538,10 +3528,10 @@
         <v>13</v>
       </c>
       <c r="D66" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E66" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F66" t="s">
         <v>16</v>
@@ -3561,7 +3551,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B67" t="s">
         <v>26</v>
@@ -3570,10 +3560,10 @@
         <v>13</v>
       </c>
       <c r="D67" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E67" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F67" t="s">
         <v>16</v>
@@ -3593,7 +3583,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B68" t="s">
         <v>26</v>
@@ -3602,10 +3592,10 @@
         <v>13</v>
       </c>
       <c r="D68" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E68" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F68" t="s">
         <v>16</v>
@@ -3625,7 +3615,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B69" t="s">
         <v>26</v>
@@ -3634,10 +3624,10 @@
         <v>13</v>
       </c>
       <c r="D69" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E69" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F69" t="s">
         <v>16</v>
@@ -3657,7 +3647,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B70" t="s">
         <v>26</v>
@@ -3666,10 +3656,10 @@
         <v>13</v>
       </c>
       <c r="D70" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E70" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F70" t="s">
         <v>16</v>
@@ -3689,19 +3679,19 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C71" t="s">
         <v>13</v>
       </c>
       <c r="D71" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E71" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F71" t="s">
         <v>16</v>
@@ -3721,7 +3711,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B72" t="s">
         <v>26</v>
@@ -3730,10 +3720,10 @@
         <v>13</v>
       </c>
       <c r="D72" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E72" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F72" t="s">
         <v>16</v>
@@ -3753,7 +3743,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B73" t="s">
         <v>26</v>
@@ -3762,10 +3752,10 @@
         <v>13</v>
       </c>
       <c r="D73" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E73" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F73" t="s">
         <v>16</v>
@@ -3785,7 +3775,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B74" t="s">
         <v>26</v>
@@ -3794,10 +3784,10 @@
         <v>13</v>
       </c>
       <c r="D74" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E74" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F74" t="s">
         <v>16</v>
@@ -3817,7 +3807,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B75" t="s">
         <v>26</v>
@@ -3826,10 +3816,10 @@
         <v>13</v>
       </c>
       <c r="D75" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E75" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F75" t="s">
         <v>16</v>
@@ -3849,7 +3839,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B76" t="s">
         <v>26</v>
@@ -3858,10 +3848,10 @@
         <v>13</v>
       </c>
       <c r="D76" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E76" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F76" t="s">
         <v>16</v>
@@ -3881,7 +3871,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B77" t="s">
         <v>26</v>
@@ -3890,10 +3880,10 @@
         <v>13</v>
       </c>
       <c r="D77" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E77" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F77" t="s">
         <v>16</v>
@@ -3913,7 +3903,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B78" t="s">
         <v>26</v>
@@ -3922,10 +3912,10 @@
         <v>13</v>
       </c>
       <c r="D78" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E78" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F78" t="s">
         <v>16</v>
@@ -3945,7 +3935,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B79" t="s">
         <v>26</v>
@@ -3954,10 +3944,10 @@
         <v>13</v>
       </c>
       <c r="D79" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E79" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F79" t="s">
         <v>16</v>
@@ -3977,7 +3967,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B80" t="s">
         <v>26</v>
@@ -3986,10 +3976,10 @@
         <v>13</v>
       </c>
       <c r="D80" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E80" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F80" t="s">
         <v>16</v>
@@ -4009,7 +3999,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B81" t="s">
         <v>26</v>
@@ -4018,10 +4008,10 @@
         <v>13</v>
       </c>
       <c r="D81" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E81" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F81" t="s">
         <v>16</v>
@@ -4041,25 +4031,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B82" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C82" t="s">
         <v>13</v>
       </c>
       <c r="D82" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E82" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F82" t="s">
         <v>16</v>
       </c>
-      <c r="G82">
-        <v>1</v>
+      <c r="G82" t="s">
+        <v>24</v>
       </c>
       <c r="I82" t="s">
         <v>18</v>
@@ -4073,7 +4063,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B83" t="s">
         <v>26</v>
@@ -4082,10 +4072,10 @@
         <v>13</v>
       </c>
       <c r="D83" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E83" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F83" t="s">
         <v>16</v>
@@ -4105,7 +4095,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B84" t="s">
         <v>26</v>
@@ -4117,7 +4107,7 @@
         <v>39</v>
       </c>
       <c r="E84" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F84" t="s">
         <v>16</v>
@@ -4137,7 +4127,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B85" t="s">
         <v>26</v>
@@ -4149,7 +4139,7 @@
         <v>39</v>
       </c>
       <c r="E85" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F85" t="s">
         <v>16</v>
@@ -4169,19 +4159,19 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B86" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C86" t="s">
         <v>13</v>
       </c>
       <c r="D86" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E86" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F86" t="s">
         <v>16</v>
@@ -4201,19 +4191,19 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>211</v>
+      </c>
+      <c r="B87" t="s">
+        <v>141</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" t="s">
+        <v>212</v>
+      </c>
+      <c r="E87" t="s">
         <v>210</v>
-      </c>
-      <c r="B87" t="s">
-        <v>140</v>
-      </c>
-      <c r="C87" t="s">
-        <v>13</v>
-      </c>
-      <c r="D87" t="s">
-        <v>211</v>
-      </c>
-      <c r="E87" t="s">
-        <v>209</v>
       </c>
       <c r="F87" t="s">
         <v>16</v>
@@ -4233,7 +4223,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B88" t="s">
         <v>26</v>
@@ -4242,10 +4232,10 @@
         <v>13</v>
       </c>
       <c r="D88" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E88" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F88" t="s">
         <v>16</v>
@@ -4265,19 +4255,19 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>216</v>
+      </c>
+      <c r="B89" t="s">
+        <v>26</v>
+      </c>
+      <c r="C89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89" t="s">
+        <v>217</v>
+      </c>
+      <c r="E89" t="s">
         <v>215</v>
-      </c>
-      <c r="B89" t="s">
-        <v>26</v>
-      </c>
-      <c r="C89" t="s">
-        <v>13</v>
-      </c>
-      <c r="D89" t="s">
-        <v>216</v>
-      </c>
-      <c r="E89" t="s">
-        <v>214</v>
       </c>
       <c r="F89" t="s">
         <v>16</v>
@@ -4297,7 +4287,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B90" t="s">
         <v>26</v>
@@ -4306,10 +4296,10 @@
         <v>13</v>
       </c>
       <c r="D90" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E90" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F90" t="s">
         <v>16</v>
@@ -4329,7 +4319,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B91" t="s">
         <v>26</v>
@@ -4338,10 +4328,10 @@
         <v>13</v>
       </c>
       <c r="D91" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E91" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F91" t="s">
         <v>16</v>
@@ -4361,7 +4351,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B92" t="s">
         <v>26</v>
@@ -4370,10 +4360,10 @@
         <v>13</v>
       </c>
       <c r="D92" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E92" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F92" t="s">
         <v>16</v>
@@ -4393,7 +4383,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B93" t="s">
         <v>26</v>
@@ -4402,10 +4392,10 @@
         <v>13</v>
       </c>
       <c r="D93" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E93" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F93" t="s">
         <v>16</v>
@@ -4425,7 +4415,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B94" t="s">
         <v>26</v>
@@ -4434,10 +4424,10 @@
         <v>13</v>
       </c>
       <c r="D94" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E94" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F94" t="s">
         <v>16</v>
@@ -4457,7 +4447,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B95" t="s">
         <v>26</v>
@@ -4466,10 +4456,10 @@
         <v>13</v>
       </c>
       <c r="D95" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E95" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F95" t="s">
         <v>16</v>
@@ -4489,7 +4479,7 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B96" t="s">
         <v>26</v>
@@ -4498,10 +4488,10 @@
         <v>13</v>
       </c>
       <c r="D96" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E96" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F96" t="s">
         <v>16</v>
@@ -4521,7 +4511,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B97" t="s">
         <v>26</v>
@@ -4530,10 +4520,10 @@
         <v>13</v>
       </c>
       <c r="D97" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E97" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F97" t="s">
         <v>16</v>
@@ -4553,7 +4543,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B98" t="s">
         <v>26</v>
@@ -4565,7 +4555,7 @@
         <v>39</v>
       </c>
       <c r="E98" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F98" t="s">
         <v>16</v>
@@ -4585,7 +4575,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B99" t="s">
         <v>26</v>
@@ -4597,7 +4587,7 @@
         <v>39</v>
       </c>
       <c r="E99" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F99" t="s">
         <v>16</v>
@@ -4617,19 +4607,19 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B100" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C100" t="s">
         <v>13</v>
       </c>
       <c r="D100" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E100" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F100" t="s">
         <v>16</v>
@@ -4649,19 +4639,19 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>239</v>
+      </c>
+      <c r="B101" t="s">
+        <v>26</v>
+      </c>
+      <c r="C101" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" t="s">
+        <v>240</v>
+      </c>
+      <c r="E101" t="s">
         <v>238</v>
-      </c>
-      <c r="B101" t="s">
-        <v>26</v>
-      </c>
-      <c r="C101" t="s">
-        <v>13</v>
-      </c>
-      <c r="D101" t="s">
-        <v>239</v>
-      </c>
-      <c r="E101" t="s">
-        <v>237</v>
       </c>
       <c r="F101" t="s">
         <v>16</v>
@@ -4681,7 +4671,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B102" t="s">
         <v>26</v>
@@ -4690,10 +4680,10 @@
         <v>13</v>
       </c>
       <c r="D102" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E102" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F102" t="s">
         <v>16</v>
@@ -4713,7 +4703,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B103" t="s">
         <v>26</v>
@@ -4722,10 +4712,10 @@
         <v>13</v>
       </c>
       <c r="D103" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E103" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F103" t="s">
         <v>16</v>
@@ -4745,7 +4735,7 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B104" t="s">
         <v>26</v>
@@ -4754,10 +4744,10 @@
         <v>13</v>
       </c>
       <c r="D104" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E104" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F104" t="s">
         <v>16</v>
@@ -4777,7 +4767,7 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B105" t="s">
         <v>26</v>
@@ -4786,10 +4776,10 @@
         <v>13</v>
       </c>
       <c r="D105" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E105" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F105" t="s">
         <v>16</v>
@@ -4809,7 +4799,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B106" t="s">
         <v>26</v>
@@ -4818,10 +4808,10 @@
         <v>13</v>
       </c>
       <c r="D106" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E106" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F106" t="s">
         <v>16</v>
@@ -4841,7 +4831,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B107" t="s">
         <v>26</v>
@@ -4850,10 +4840,10 @@
         <v>13</v>
       </c>
       <c r="D107" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E107" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F107" t="s">
         <v>16</v>
@@ -4873,19 +4863,19 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>255</v>
+      </c>
+      <c r="B108" t="s">
+        <v>26</v>
+      </c>
+      <c r="C108" t="s">
+        <v>13</v>
+      </c>
+      <c r="D108" t="s">
+        <v>256</v>
+      </c>
+      <c r="E108" t="s">
         <v>254</v>
-      </c>
-      <c r="B108" t="s">
-        <v>26</v>
-      </c>
-      <c r="C108" t="s">
-        <v>13</v>
-      </c>
-      <c r="D108" t="s">
-        <v>255</v>
-      </c>
-      <c r="E108" t="s">
-        <v>253</v>
       </c>
       <c r="F108" t="s">
         <v>16</v>
@@ -4905,7 +4895,7 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B109" t="s">
         <v>26</v>
@@ -4914,10 +4904,10 @@
         <v>13</v>
       </c>
       <c r="D109" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E109" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F109" t="s">
         <v>16</v>
@@ -4937,7 +4927,7 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B110" t="s">
         <v>26</v>
@@ -4946,10 +4936,10 @@
         <v>13</v>
       </c>
       <c r="D110" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E110" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F110" t="s">
         <v>16</v>
@@ -4969,7 +4959,7 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B111" t="s">
         <v>26</v>
@@ -4978,10 +4968,10 @@
         <v>13</v>
       </c>
       <c r="D111" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E111" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F111" t="s">
         <v>16</v>
@@ -5001,25 +4991,25 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>264</v>
+      </c>
+      <c r="B112" t="s">
+        <v>26</v>
+      </c>
+      <c r="C112" t="s">
+        <v>13</v>
+      </c>
+      <c r="D112" t="s">
+        <v>265</v>
+      </c>
+      <c r="E112" t="s">
         <v>263</v>
       </c>
-      <c r="B112" t="s">
-        <v>26</v>
-      </c>
-      <c r="C112" t="s">
-        <v>13</v>
-      </c>
-      <c r="D112" t="s">
-        <v>264</v>
-      </c>
-      <c r="E112" t="s">
-        <v>262</v>
-      </c>
       <c r="F112" t="s">
         <v>16</v>
       </c>
-      <c r="G112">
-        <v>1</v>
+      <c r="G112" t="s">
+        <v>17</v>
       </c>
       <c r="I112" t="s">
         <v>18</v>
@@ -5033,7 +5023,7 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B113" t="s">
         <v>26</v>
@@ -5045,7 +5035,7 @@
         <v>39</v>
       </c>
       <c r="E113" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F113" t="s">
         <v>16</v>
@@ -5065,7 +5055,7 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B114" t="s">
         <v>30</v>
@@ -5074,10 +5064,10 @@
         <v>13</v>
       </c>
       <c r="D114" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E114" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F114" t="s">
         <v>16</v>
@@ -5092,44 +5082,44 @@
         <v>19</v>
       </c>
       <c r="K114" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>272</v>
+      </c>
+      <c r="B115" t="s">
+        <v>26</v>
+      </c>
+      <c r="C115" t="s">
+        <v>13</v>
+      </c>
+      <c r="D115" t="s">
+        <v>273</v>
+      </c>
+      <c r="E115" t="s">
+        <v>270</v>
+      </c>
+      <c r="F115" t="s">
+        <v>16</v>
+      </c>
+      <c r="G115" t="s">
+        <v>24</v>
+      </c>
+      <c r="I115" t="s">
+        <v>18</v>
+      </c>
+      <c r="J115" t="s">
+        <v>19</v>
+      </c>
+      <c r="K115" t="s">
         <v>271</v>
-      </c>
-      <c r="B115" t="s">
-        <v>26</v>
-      </c>
-      <c r="C115" t="s">
-        <v>13</v>
-      </c>
-      <c r="D115" t="s">
-        <v>272</v>
-      </c>
-      <c r="E115" t="s">
-        <v>269</v>
-      </c>
-      <c r="F115" t="s">
-        <v>16</v>
-      </c>
-      <c r="G115" t="s">
-        <v>24</v>
-      </c>
-      <c r="I115" t="s">
-        <v>18</v>
-      </c>
-      <c r="J115" t="s">
-        <v>19</v>
-      </c>
-      <c r="K115" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B116" t="s">
         <v>26</v>
@@ -5138,10 +5128,10 @@
         <v>13</v>
       </c>
       <c r="D116" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E116" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F116" t="s">
         <v>16</v>
@@ -5156,12 +5146,12 @@
         <v>19</v>
       </c>
       <c r="K116" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B117" t="s">
         <v>26</v>
@@ -5170,10 +5160,10 @@
         <v>13</v>
       </c>
       <c r="D117" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E117" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F117" t="s">
         <v>16</v>
@@ -5188,12 +5178,12 @@
         <v>19</v>
       </c>
       <c r="K117" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B118" t="s">
         <v>26</v>
@@ -5202,10 +5192,10 @@
         <v>13</v>
       </c>
       <c r="D118" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E118" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F118" t="s">
         <v>16</v>
@@ -5220,12 +5210,12 @@
         <v>19</v>
       </c>
       <c r="K118" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B119" t="s">
         <v>26</v>
@@ -5234,10 +5224,10 @@
         <v>13</v>
       </c>
       <c r="D119" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E119" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F119" t="s">
         <v>16</v>
@@ -5252,12 +5242,12 @@
         <v>19</v>
       </c>
       <c r="K119" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B120" t="s">
         <v>26</v>
@@ -5266,10 +5256,10 @@
         <v>13</v>
       </c>
       <c r="D120" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E120" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F120" t="s">
         <v>16</v>
@@ -5284,25 +5274,25 @@
         <v>19</v>
       </c>
       <c r="K120" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>285</v>
+      </c>
+      <c r="B121" t="s">
+        <v>26</v>
+      </c>
+      <c r="C121" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121" t="s">
+        <v>286</v>
+      </c>
+      <c r="E121" t="s">
         <v>284</v>
       </c>
-      <c r="B121" t="s">
-        <v>26</v>
-      </c>
-      <c r="C121" t="s">
-        <v>13</v>
-      </c>
-      <c r="D121" t="s">
-        <v>285</v>
-      </c>
-      <c r="E121" t="s">
-        <v>283</v>
-      </c>
       <c r="F121" t="s">
         <v>16</v>
       </c>
@@ -5316,12 +5306,12 @@
         <v>19</v>
       </c>
       <c r="K121" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B122" t="s">
         <v>26</v>
@@ -5330,10 +5320,10 @@
         <v>13</v>
       </c>
       <c r="D122" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E122" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F122" t="s">
         <v>16</v>
@@ -5348,12 +5338,12 @@
         <v>19</v>
       </c>
       <c r="K122" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B123" t="s">
         <v>26</v>
@@ -5362,10 +5352,10 @@
         <v>13</v>
       </c>
       <c r="D123" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E123" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F123" t="s">
         <v>16</v>
@@ -5380,44 +5370,44 @@
         <v>19</v>
       </c>
       <c r="K123" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
+        <v>293</v>
+      </c>
+      <c r="B124" t="s">
+        <v>141</v>
+      </c>
+      <c r="C124" t="s">
+        <v>13</v>
+      </c>
+      <c r="D124" t="s">
+        <v>294</v>
+      </c>
+      <c r="E124" t="s">
+        <v>291</v>
+      </c>
+      <c r="F124" t="s">
+        <v>16</v>
+      </c>
+      <c r="G124" t="s">
+        <v>24</v>
+      </c>
+      <c r="I124" t="s">
+        <v>18</v>
+      </c>
+      <c r="J124" t="s">
+        <v>19</v>
+      </c>
+      <c r="K124" t="s">
         <v>292</v>
-      </c>
-      <c r="B124" t="s">
-        <v>140</v>
-      </c>
-      <c r="C124" t="s">
-        <v>13</v>
-      </c>
-      <c r="D124" t="s">
-        <v>293</v>
-      </c>
-      <c r="E124" t="s">
-        <v>290</v>
-      </c>
-      <c r="F124" t="s">
-        <v>16</v>
-      </c>
-      <c r="G124" t="s">
-        <v>24</v>
-      </c>
-      <c r="I124" t="s">
-        <v>18</v>
-      </c>
-      <c r="J124" t="s">
-        <v>19</v>
-      </c>
-      <c r="K124" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B125" t="s">
         <v>26</v>
@@ -5426,10 +5416,10 @@
         <v>13</v>
       </c>
       <c r="D125" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E125" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F125" t="s">
         <v>16</v>
@@ -5444,12 +5434,12 @@
         <v>19</v>
       </c>
       <c r="K125" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B126" t="s">
         <v>26</v>
@@ -5458,10 +5448,10 @@
         <v>13</v>
       </c>
       <c r="D126" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E126" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F126" t="s">
         <v>16</v>
@@ -5476,12 +5466,12 @@
         <v>19</v>
       </c>
       <c r="K126" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B127" t="s">
         <v>26</v>
@@ -5490,10 +5480,10 @@
         <v>13</v>
       </c>
       <c r="D127" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E127" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F127" t="s">
         <v>16</v>
@@ -5508,12 +5498,12 @@
         <v>19</v>
       </c>
       <c r="K127" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B128" t="s">
         <v>26</v>
@@ -5522,10 +5512,10 @@
         <v>13</v>
       </c>
       <c r="D128" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E128" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F128" t="s">
         <v>16</v>
@@ -5540,12 +5530,12 @@
         <v>19</v>
       </c>
       <c r="K128" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B129" t="s">
         <v>26</v>
@@ -5554,10 +5544,10 @@
         <v>13</v>
       </c>
       <c r="D129" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E129" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F129" t="s">
         <v>16</v>
@@ -5572,25 +5562,25 @@
         <v>19</v>
       </c>
       <c r="K129" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>306</v>
+      </c>
+      <c r="B130" t="s">
+        <v>26</v>
+      </c>
+      <c r="C130" t="s">
+        <v>13</v>
+      </c>
+      <c r="D130" t="s">
+        <v>307</v>
+      </c>
+      <c r="E130" t="s">
         <v>305</v>
       </c>
-      <c r="B130" t="s">
-        <v>26</v>
-      </c>
-      <c r="C130" t="s">
-        <v>13</v>
-      </c>
-      <c r="D130" t="s">
-        <v>306</v>
-      </c>
-      <c r="E130" t="s">
-        <v>304</v>
-      </c>
       <c r="F130" t="s">
         <v>16</v>
       </c>
@@ -5604,12 +5594,12 @@
         <v>19</v>
       </c>
       <c r="K130" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B131" t="s">
         <v>26</v>
@@ -5618,10 +5608,10 @@
         <v>13</v>
       </c>
       <c r="D131" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E131" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F131" t="s">
         <v>16</v>
@@ -5636,44 +5626,44 @@
         <v>19</v>
       </c>
       <c r="K131" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>312</v>
+      </c>
+      <c r="B132" t="s">
+        <v>26</v>
+      </c>
+      <c r="C132" t="s">
+        <v>13</v>
+      </c>
+      <c r="D132" t="s">
+        <v>313</v>
+      </c>
+      <c r="E132" t="s">
+        <v>310</v>
+      </c>
+      <c r="F132" t="s">
+        <v>16</v>
+      </c>
+      <c r="G132" t="s">
+        <v>24</v>
+      </c>
+      <c r="I132" t="s">
+        <v>18</v>
+      </c>
+      <c r="J132" t="s">
+        <v>19</v>
+      </c>
+      <c r="K132" t="s">
         <v>311</v>
-      </c>
-      <c r="B132" t="s">
-        <v>26</v>
-      </c>
-      <c r="C132" t="s">
-        <v>13</v>
-      </c>
-      <c r="D132" t="s">
-        <v>312</v>
-      </c>
-      <c r="E132" t="s">
-        <v>309</v>
-      </c>
-      <c r="F132" t="s">
-        <v>16</v>
-      </c>
-      <c r="G132" t="s">
-        <v>24</v>
-      </c>
-      <c r="I132" t="s">
-        <v>18</v>
-      </c>
-      <c r="J132" t="s">
-        <v>19</v>
-      </c>
-      <c r="K132" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B133" t="s">
         <v>26</v>
@@ -5682,10 +5672,10 @@
         <v>13</v>
       </c>
       <c r="D133" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E133" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F133" t="s">
         <v>16</v>
@@ -5700,12 +5690,12 @@
         <v>19</v>
       </c>
       <c r="K133" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B134" t="s">
         <v>26</v>
@@ -5714,10 +5704,10 @@
         <v>13</v>
       </c>
       <c r="D134" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E134" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F134" t="s">
         <v>16</v>
@@ -5732,12 +5722,12 @@
         <v>19</v>
       </c>
       <c r="K134" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B135" t="s">
         <v>26</v>
@@ -5746,10 +5736,10 @@
         <v>13</v>
       </c>
       <c r="D135" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E135" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F135" t="s">
         <v>16</v>
@@ -5764,44 +5754,44 @@
         <v>19</v>
       </c>
       <c r="K135" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>323</v>
+      </c>
+      <c r="B136" t="s">
+        <v>26</v>
+      </c>
+      <c r="C136" t="s">
+        <v>13</v>
+      </c>
+      <c r="D136" t="s">
+        <v>324</v>
+      </c>
+      <c r="E136" t="s">
+        <v>321</v>
+      </c>
+      <c r="F136" t="s">
+        <v>16</v>
+      </c>
+      <c r="G136" t="s">
+        <v>24</v>
+      </c>
+      <c r="I136" t="s">
+        <v>18</v>
+      </c>
+      <c r="J136" t="s">
+        <v>19</v>
+      </c>
+      <c r="K136" t="s">
         <v>322</v>
-      </c>
-      <c r="B136" t="s">
-        <v>26</v>
-      </c>
-      <c r="C136" t="s">
-        <v>13</v>
-      </c>
-      <c r="D136" t="s">
-        <v>323</v>
-      </c>
-      <c r="E136" t="s">
-        <v>320</v>
-      </c>
-      <c r="F136" t="s">
-        <v>16</v>
-      </c>
-      <c r="G136" t="s">
-        <v>24</v>
-      </c>
-      <c r="I136" t="s">
-        <v>18</v>
-      </c>
-      <c r="J136" t="s">
-        <v>19</v>
-      </c>
-      <c r="K136" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B137" t="s">
         <v>26</v>
@@ -5810,10 +5800,10 @@
         <v>13</v>
       </c>
       <c r="D137" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E137" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F137" t="s">
         <v>16</v>
@@ -5828,12 +5818,12 @@
         <v>19</v>
       </c>
       <c r="K137" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B138" t="s">
         <v>26</v>
@@ -5842,10 +5832,10 @@
         <v>13</v>
       </c>
       <c r="D138" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E138" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F138" t="s">
         <v>16</v>
@@ -5860,12 +5850,12 @@
         <v>19</v>
       </c>
       <c r="K138" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B139" t="s">
         <v>26</v>
@@ -5874,10 +5864,10 @@
         <v>13</v>
       </c>
       <c r="D139" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E139" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F139" t="s">
         <v>16</v>
@@ -5892,25 +5882,25 @@
         <v>19</v>
       </c>
       <c r="K139" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>332</v>
+      </c>
+      <c r="B140" t="s">
+        <v>26</v>
+      </c>
+      <c r="C140" t="s">
+        <v>13</v>
+      </c>
+      <c r="D140" t="s">
+        <v>333</v>
+      </c>
+      <c r="E140" t="s">
         <v>331</v>
       </c>
-      <c r="B140" t="s">
-        <v>26</v>
-      </c>
-      <c r="C140" t="s">
-        <v>13</v>
-      </c>
-      <c r="D140" t="s">
-        <v>332</v>
-      </c>
-      <c r="E140" t="s">
-        <v>330</v>
-      </c>
       <c r="F140" t="s">
         <v>16</v>
       </c>
@@ -5924,12 +5914,12 @@
         <v>19</v>
       </c>
       <c r="K140" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B141" t="s">
         <v>26</v>
@@ -5938,10 +5928,10 @@
         <v>13</v>
       </c>
       <c r="D141" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E141" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F141" t="s">
         <v>16</v>
@@ -5956,24 +5946,24 @@
         <v>19</v>
       </c>
       <c r="K141" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B142" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C142" t="s">
         <v>13</v>
       </c>
       <c r="D142" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E142" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F142" t="s">
         <v>16</v>
@@ -5988,24 +5978,24 @@
         <v>19</v>
       </c>
       <c r="K142" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B143" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C143" t="s">
+        <v>339</v>
+      </c>
+      <c r="D143" t="s">
+        <v>340</v>
+      </c>
+      <c r="E143" t="s">
         <v>338</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="E143" t="s">
-        <v>337</v>
       </c>
       <c r="F143" t="s">
         <v>16</v>
@@ -6014,7 +6004,7 @@
         <v>17</v>
       </c>
       <c r="I143" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="J143" t="s">
         <v>19</v>
@@ -6024,13 +6014,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D16" r:id="rId1" xr:uid="{F626E72E-66E9-489F-AD07-DBB28F3BF3DA}"/>
-    <hyperlink ref="D18" r:id="rId2" xr:uid="{A8F3035A-216D-4732-8AC6-DF32AF383FB7}"/>
-    <hyperlink ref="D143" r:id="rId3" xr:uid="{4BEFA9D6-41A5-46CB-B6B9-E9B2AA1CC315}"/>
-    <hyperlink ref="D15" r:id="rId4" xr:uid="{C9A3ED06-A98F-4442-9685-171E27A779E1}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>